<commit_message>
Update R scripts and data.
</commit_message>
<xml_diff>
--- a/01_data/lookup_tables/summary_of_robustness_tests-2025-01-09.xlsx
+++ b/01_data/lookup_tables/summary_of_robustness_tests-2025-01-09.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Seagate/eCommerce-Goethe Dropbox/Karlo Lukic/01-doctorate/00_research_projects/01_impact_of_GDPR_on_online_tracking/08_tables_and_figures/table_08_summary_of_robustness_tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karlolukic/Documents/impact-of-GDPR-on-online-tracking-2025-01-10/01_data/lookup_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD572182-2D53-7649-8ECC-1157D2FC6FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D245E2D-B1DC-884C-B27B-011BE181C80A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="18700" xr2:uid="{0B5DA345-615C-F144-970C-B479B0992921}"/>
   </bookViews>
@@ -171,7 +171,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -185,6 +185,20 @@
       <family val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -211,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -225,6 +239,11 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -562,7 +581,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -574,17 +593,17 @@
     <col min="5" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" s="9" customFormat="1" ht="17">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="8" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>